<commit_message>
Add latest Excel template
</commit_message>
<xml_diff>
--- a/templates/voc4cat_template_043.xlsx
+++ b/templates/voc4cat_template_043.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\nfdi4cat\gh-dalito\voc4cat-template\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\gh-nfdi4cat\voc4cat-template\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D4E7DC-20C2-4CA2-B23B-F550D63A5BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5279714C-CB90-44D9-8E9A-A63F98EB4A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -210,9 +210,6 @@
     <t>https://example.org/new/</t>
   </si>
   <si>
-    <t>https://w3id.org/nfdi4cat/voc4cat/</t>
-  </si>
-  <si>
     <t>The spreadsheet is processed with voc4cat which extends vocexcel for the voc4cat-based repositories.</t>
   </si>
   <si>
@@ -1243,9 +1240,6 @@
   </si>
   <si>
     <t>revision</t>
-  </si>
-  <si>
-    <t>2023-03a</t>
   </si>
   <si>
     <r>
@@ -1574,6 +1568,12 @@
   </si>
   <si>
     <t>Concepts*</t>
+  </si>
+  <si>
+    <t>https://w3id.org/nfdi4cat/voc4cat_</t>
+  </si>
+  <si>
+    <t>2023-06a</t>
   </si>
 </sst>
 </file>
@@ -1914,66 +1914,6 @@
   </cellStyles>
   <dxfs count="26">
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FFD9EAD3"/>
       </font>
@@ -2038,6 +1978,66 @@
           <bgColor rgb="FFD9EAD3"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2110,25 +2110,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8DAB75F9-D01E-4902-B5DF-39342F86B90D}" name="concepts" displayName="concepts" ref="A2:I20" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8DAB75F9-D01E-4902-B5DF-39342F86B90D}" name="concepts" displayName="concepts" ref="A2:I20" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A2:I20" xr:uid="{8DAB75F9-D01E-4902-B5DF-39342F86B90D}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{9FE8BFF8-A78B-448D-A131-9A0D98C9F3D7}" name="Concept IRI*" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{86239A34-9941-49E0-9977-1A07DF28C21F}" name="Preferred Label*" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{3DDC515C-66BD-4D72-9F90-11ECCC367C9E}" name="Pref. Label Language Code" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{DFD56705-3476-4395-8E82-4BA1B2D9FB6C}" name="Definition*" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{73464C4B-4966-4F01-A700-A547FE1A016C}" name="Def. Language Code" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{A1F0E882-A632-4EAB-9875-D263174AB2AC}" name="Alternate Labels" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{45F1B146-1861-40A5-A017-E62DF2AF1EDE}" name="Children IRIs" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{6CD00781-D481-43C6-9E4B-C9105CE6954A}" name="Provenance*" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{C6B9560F-7DE1-43A3-AE9F-6EEE88487995}" name="Source Vocab URI" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{9FE8BFF8-A78B-448D-A131-9A0D98C9F3D7}" name="Concept IRI*" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{86239A34-9941-49E0-9977-1A07DF28C21F}" name="Preferred Label*" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{3DDC515C-66BD-4D72-9F90-11ECCC367C9E}" name="Pref. Label Language Code" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{DFD56705-3476-4395-8E82-4BA1B2D9FB6C}" name="Definition*" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{73464C4B-4966-4F01-A700-A547FE1A016C}" name="Def. Language Code" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{A1F0E882-A632-4EAB-9875-D263174AB2AC}" name="Alternate Labels" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{45F1B146-1861-40A5-A017-E62DF2AF1EDE}" name="Children IRIs" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{6CD00781-D481-43C6-9E4B-C9105CE6954A}" name="Provenance*" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{C6B9560F-7DE1-43A3-AE9F-6EEE88487995}" name="Source Vocab URI" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F0019B54-5478-4B2D-B2DC-B81783F2E087}" name="concept_relations" displayName="concept_relations" ref="A2:F20" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F0019B54-5478-4B2D-B2DC-B81783F2E087}" name="concept_relations" displayName="concept_relations" ref="A2:F20" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="A2:F20" xr:uid="{F0019B54-5478-4B2D-B2DC-B81783F2E087}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{94539CED-3865-4A8C-AC09-EF3C512E3567}" name="Concept IRI*"/>
@@ -2143,21 +2143,21 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6ED60B90-A5EC-4F1E-9CF2-D984C20452D6}" name="collections" displayName="collections" ref="A2:E20" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6ED60B90-A5EC-4F1E-9CF2-D984C20452D6}" name="collections" displayName="collections" ref="A2:E20" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A2:E20" xr:uid="{6ED60B90-A5EC-4F1E-9CF2-D984C20452D6}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{93EAAE4B-8D60-4F74-8745-A2195B7A0D5C}" name="Collection IRI" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{134406ED-31FC-425A-82E8-23EE8F1B82A5}" name="Preferred Label" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{CA3ED009-9BFA-4919-9F93-47D10664A305}" name="Definition" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{E52278B9-419C-4E49-BF0A-3898B2077694}" name="Member IRIs" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{E12774E7-E938-4E4B-A0FF-F29983D1E4C6}" name="Provenance" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{93EAAE4B-8D60-4F74-8745-A2195B7A0D5C}" name="Collection IRI" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{134406ED-31FC-425A-82E8-23EE8F1B82A5}" name="Preferred Label" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{CA3ED009-9BFA-4919-9F93-47D10664A305}" name="Definition" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{E52278B9-419C-4E49-BF0A-3898B2077694}" name="Member IRIs" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{E12774E7-E938-4E4B-A0FF-F29983D1E4C6}" name="Provenance" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0A8562A3-BEFF-43D4-B887-56FC0330A95A}" name="prefixes" displayName="prefixes" ref="A1:B20" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0A8562A3-BEFF-43D4-B887-56FC0330A95A}" name="prefixes" displayName="prefixes" ref="A1:B20" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A1:B20" xr:uid="{0A8562A3-BEFF-43D4-B887-56FC0330A95A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A30D4DF8-3B4A-4F43-9882-EDFDD8090F9E}" name="Prefix"/>
@@ -2469,7 +2469,9 @@
   </sheetPr>
   <dimension ref="A11:L31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2486,7 +2488,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="3"/>
       <c r="I11" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>0</v>
@@ -2495,15 +2497,15 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H12" s="24"/>
       <c r="I12" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14" s="27"/>
       <c r="D14" s="27"/>
@@ -2564,12 +2566,12 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D22" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>32</v>
@@ -2577,7 +2579,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D23" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E23" s="10" t="s">
         <v>34</v>
@@ -2585,10 +2587,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D24" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2596,29 +2598,29 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D26" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D27" s="8"/>
       <c r="E27" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D31" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2658,7 +2660,7 @@
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -2726,7 +2728,7 @@
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2739,10 +2741,10 @@
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="20"/>
       <c r="C9" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="5"/>
@@ -2752,10 +2754,10 @@
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="C10" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="5"/>
@@ -2776,7 +2778,7 @@
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="27"/>
@@ -3151,7 +3153,7 @@
     </row>
     <row r="46" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B46" s="27" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C46" s="27"/>
       <c r="D46" s="27"/>
@@ -3605,7 +3607,7 @@
     <row r="87" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="88" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B88" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C88" s="27"/>
       <c r="D88" s="27"/>
@@ -3905,7 +3907,7 @@
     <row r="115" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="116" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B116" s="27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C116" s="27"/>
       <c r="D116" s="27"/>
@@ -4062,7 +4064,7 @@
     <row r="130" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="131" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B131" s="27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C131" s="27"/>
       <c r="D131" s="27"/>
@@ -4186,7 +4188,7 @@
     <row r="142" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="143" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B143" s="28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C143" s="28"/>
       <c r="D143" s="28"/>
@@ -4243,18 +4245,18 @@
     </row>
     <row r="148" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D148" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="E148" s="10" t="s">
         <v>101</v>
-      </c>
-      <c r="E148" s="10" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="149" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D149" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E149" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="150" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
@@ -5289,32 +5291,32 @@
     <mergeCell ref="B116:J129"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:B4 B46:B86">
-    <cfRule type="containsBlanks" dxfId="25" priority="7">
+    <cfRule type="containsBlanks" dxfId="5" priority="7">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B44">
-    <cfRule type="containsBlanks" dxfId="24" priority="6">
+    <cfRule type="containsBlanks" dxfId="4" priority="6">
       <formula>LEN(TRIM(B12))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88">
-    <cfRule type="containsBlanks" dxfId="23" priority="4">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(B88))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B116">
-    <cfRule type="containsBlanks" dxfId="22" priority="3">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(B116))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B131">
-    <cfRule type="containsBlanks" dxfId="21" priority="2">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(B131))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B143:B147">
-    <cfRule type="containsBlanks" dxfId="20" priority="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(B143))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5350,7 +5352,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -5358,10 +5360,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>30</v>
@@ -5372,10 +5374,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>3</v>
@@ -5386,10 +5388,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>3</v>
@@ -5403,10 +5405,10 @@
         <v>44995</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5417,10 +5419,10 @@
         <v>44995</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5431,10 +5433,10 @@
         <v>29</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5445,10 +5447,10 @@
         <v>29</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -5456,10 +5458,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>108</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>109</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>10</v>
@@ -5470,7 +5472,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>12</v>
@@ -5484,7 +5486,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>14</v>
@@ -6519,7 +6521,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -6530,19 +6532,19 @@
         <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
@@ -6553,78 +6555,78 @@
     </row>
     <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>68</v>
-      </c>
       <c r="D3" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I3" s="9"/>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>74</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>82</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>83</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I5" s="9"/>
     </row>
@@ -6825,7 +6827,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -6833,27 +6835,27 @@
         <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25"/>
@@ -7383,7 +7385,7 @@
         <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>21</v>
@@ -7391,19 +7393,19 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -7579,7 +7581,7 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -7591,7 +7593,7 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{721C34C9-12AA-45FE-91A4-8BCB1AB59BCB}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{0E392E66-5F6B-4692-BC52-7DAF5D46D4EA}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://w3id.org/nfdi4cat/voc4cat/" xr:uid="{0E392E66-5F6B-4692-BC52-7DAF5D46D4EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>